<commit_message>
added read testdata code
</commit_message>
<xml_diff>
--- a/TestData/HRM_TestData.xlsx
+++ b/TestData/HRM_TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91770\eclipse-workspace\Automation_Framework_May2020\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2364CAB8-5CF2-400C-930F-389A3BA4D5CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F891FAB5-27FC-4785-96AD-B7A37255ECC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A26426-1E60-4407-BDCF-BA3E2BDF78E7}"/>
   </bookViews>
@@ -31,9 +31,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>TestCase_Name</t>
+  </si>
+  <si>
+    <t>tc001_VerifyLoginAuthentication</t>
+  </si>
+  <si>
+    <t>tc002_ApplyLeave</t>
+  </si>
+  <si>
+    <t>tc003_CancelLeave</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>user02</t>
+  </si>
+  <si>
+    <t>user03</t>
+  </si>
+  <si>
+    <t>user04</t>
+  </si>
+  <si>
+    <t>TM1234</t>
+  </si>
+  <si>
+    <t>TM1235</t>
+  </si>
+  <si>
+    <t>TM1236</t>
+  </si>
+  <si>
+    <t>Annual Leave</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,16 +85,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -58,12 +121,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,15 +462,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4E8AE0-BF8D-4E7A-A4EE-EE52A2F885EF}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6">
+        <v>44037</v>
+      </c>
+      <c r="G3" s="6">
+        <v>44038</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
HashMap to read testdata
</commit_message>
<xml_diff>
--- a/TestData/HRM_TestData.xlsx
+++ b/TestData/HRM_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91770\eclipse-workspace\Automation_Framework_May2020\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F891FAB5-27FC-4785-96AD-B7A37255ECC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7325E426-CC1F-4516-BA03-9665924B61DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53A26426-1E60-4407-BDCF-BA3E2BDF78E7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TestCase_Name</t>
   </si>
@@ -49,28 +49,34 @@
     <t>#</t>
   </si>
   <si>
-    <t>user02</t>
-  </si>
-  <si>
-    <t>user03</t>
-  </si>
-  <si>
-    <t>user04</t>
-  </si>
-  <si>
-    <t>TM1234</t>
-  </si>
-  <si>
-    <t>TM1235</t>
-  </si>
-  <si>
-    <t>TM1236</t>
-  </si>
-  <si>
-    <t>Annual Leave</t>
-  </si>
-  <si>
-    <t>Function</t>
+    <t>pwd:=TM1234</t>
+  </si>
+  <si>
+    <t>pwd:=TM1235</t>
+  </si>
+  <si>
+    <t>pwd:=TM1236</t>
+  </si>
+  <si>
+    <t>leaveType:=Annual Leave</t>
+  </si>
+  <si>
+    <t>user:=user02</t>
+  </si>
+  <si>
+    <t>user:=user03</t>
+  </si>
+  <si>
+    <t>user:=user04</t>
+  </si>
+  <si>
+    <t>fromDate:=25-07-2020</t>
+  </si>
+  <si>
+    <t>toDate:=26-07-2020</t>
+  </si>
+  <si>
+    <t>comment:=attend function</t>
   </si>
 </sst>
 </file>
@@ -92,7 +98,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -142,12 +148,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,36 +471,37 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -502,17 +509,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -520,25 +527,25 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6">
-        <v>44037</v>
-      </c>
-      <c r="G3" s="6">
-        <v>44038</v>
+        <v>8</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -546,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>

</xml_diff>